<commit_message>
button fix + SQL database update
</commit_message>
<xml_diff>
--- a/diagrams/SQLPlan.xlsx
+++ b/diagrams/SQLPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szena\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProjektOKJ\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9A5CC2-1D54-4BE7-B0C2-864D02568414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF5FC89-A01F-43B9-A0CC-4D5F799A9424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{09CBA4D3-A3FF-4421-9EAC-9E3D4B6FD877}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Users</t>
   </si>
@@ -97,6 +97,57 @@
   </si>
   <si>
     <t>userAdmin - bit(1)</t>
+  </si>
+  <si>
+    <t>gamePic - varchar(255)</t>
+  </si>
+  <si>
+    <t>Minimum Requirements</t>
+  </si>
+  <si>
+    <t>Recommended Requirements</t>
+  </si>
+  <si>
+    <t>mGId - FOREIGN KEY - Games</t>
+  </si>
+  <si>
+    <t>rGId - FOREIGN KEY - Games</t>
+  </si>
+  <si>
+    <t>minimumId - int(11) - PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>recommendedId - int(11) - PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>mOS - varchar(255)</t>
+  </si>
+  <si>
+    <t>mProcessor - varchar(255)</t>
+  </si>
+  <si>
+    <t>mMemory - varchar(255)</t>
+  </si>
+  <si>
+    <t>mGPU - varchar(255)</t>
+  </si>
+  <si>
+    <t>mStorage- varchar(255)</t>
+  </si>
+  <si>
+    <t>rOS - varchar(255)</t>
+  </si>
+  <si>
+    <t>rProcessor - varchar(255)</t>
+  </si>
+  <si>
+    <t>rMemory - varchar(255)</t>
+  </si>
+  <si>
+    <t>rGPU - varchar(255)</t>
+  </si>
+  <si>
+    <t>rStorage- varchar(255)</t>
   </si>
 </sst>
 </file>
@@ -128,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -151,32 +202,197 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -491,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB61A62-1D0C-4230-B58B-2D2289BC22C8}">
-  <dimension ref="B2:Q21"/>
+  <dimension ref="B2:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,243 +721,386 @@
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="13" max="13" width="17.140625" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="24" max="24" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="14"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="15"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="18"/>
+    </row>
+    <row r="5" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3" t="s">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="O5" s="5"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="10"/>
+    </row>
+    <row r="6" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+    </row>
+    <row r="7" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3" t="s">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="O7" s="5"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+    </row>
+    <row r="8" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+      <c r="Q8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+    </row>
+    <row r="9" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="2:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="Q9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="22"/>
+    </row>
+    <row r="10" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="12:17" x14ac:dyDescent="0.25">
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="12:17" x14ac:dyDescent="0.25">
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="Q10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="22"/>
+    </row>
+    <row r="11" spans="2:24" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="Q11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="22"/>
+      <c r="U11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="22"/>
+    </row>
+    <row r="16" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+    </row>
+    <row r="17" spans="12:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+    </row>
+    <row r="18" spans="12:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
     </row>
     <row r="19" spans="12:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="12:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
     </row>
     <row r="21" spans="12:17" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="41">
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="U10:X10"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="U2:X4"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="Q2:T4"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K2:M4"/>
+    <mergeCell ref="N2:P4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="Q9:T9"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="N7:P7"/>
@@ -755,26 +1114,9 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="O16:Q18"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="O21:Q21"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="H2:J4"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K2:M4"/>
-    <mergeCell ref="N2:P4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="L16:N18"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="L21:N21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>